<commit_message>
update: gitbook version up
</commit_message>
<xml_diff>
--- a/data-raw/fig-tab.xlsx
+++ b/data-raw/fig-tab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmc\pipetbooks\basic\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047818CC-E8E3-4E53-9920-72697B36E67C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FF2264-58A2-4DF1-B038-D528E5EC6D1F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-5670" windowWidth="16440" windowHeight="28440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="245">
   <si>
     <t>Variable Name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -244,17 +244,6 @@
     <t>Bioavailability for Peripheral compartment</t>
   </si>
   <si>
-    <t>Starting Value: 0.70</t>
-  </si>
-  <si>
-    <t>i</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Starting Value: 1.60</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>ㅿParameters</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -272,9 +261,6 @@
     <t>readxl::read_excel("data-raw/fig-tab.xlsx", sheet="50", range="B2:E36")</t>
   </si>
   <si>
-    <t>readxl::read_excel("data-raw/fig-tab.xlsx", sheet="71", range="B2:F20")</t>
-  </si>
-  <si>
     <t>readxl::read_excel("data-raw/fig-tab.xlsx", sheet="125", range="B2:C6")</t>
   </si>
   <si>
@@ -792,18 +778,40 @@
   </si>
   <si>
     <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>xi</t>
+  </si>
+  <si>
+    <t>dydxi</t>
+  </si>
+  <si>
+    <t>dyd2xi</t>
+  </si>
+  <si>
+    <t>xi+1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starting </t>
+  </si>
+  <si>
+    <t>Value: 1.60</t>
+  </si>
+  <si>
+    <t>Value: 0.70</t>
+  </si>
+  <si>
+    <t>readxl::read_excel("data-raw/fig-tab.xlsx", sheet="71", range="B2:F19")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.00_);[Red]\(0.00\)"/>
-  </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -850,14 +858,6 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -897,15 +897,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -933,36 +930,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
+  <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1310,669 +1282,18 @@
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>277881</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>23397</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="240322" cy="350032"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="TextBox 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2340251" y="230462"/>
-              <a:ext cx="240322" cy="350032"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:f>
-                      <m:fPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:fPr>
-                      <m:num>
-                        <m:r>
-                          <a:rPr lang="ko-KR" altLang="en-US" sz="1100">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>ⅆ</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑌</m:t>
-                        </m:r>
-                      </m:num>
-                      <m:den>
-                        <m:r>
-                          <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="0">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>ⅆ</m:t>
-                        </m:r>
-                        <m:sSub>
-                          <m:sSubPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:sSubPr>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>𝑋</m:t>
-                            </m:r>
-                          </m:e>
-                          <m:sub>
-                            <m:r>
-                              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>𝑖</m:t>
-                            </m:r>
-                          </m:sub>
-                        </m:sSub>
-                      </m:den>
-                    </m:f>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="TextBox 1"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2340251" y="230462"/>
-              <a:ext cx="240322" cy="350032"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>ⅆ𝑌/(ⅆ𝑋_𝑖 )</a:t>
-              </a:r>
-              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>288234</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>110158</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="162096" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="TextBox 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="1663147" y="317223"/>
-              <a:ext cx="162096" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑋</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑖</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="TextBox 2"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="1663147" y="317223"/>
-              <a:ext cx="162096" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑋_𝑖</a:t>
-              </a:r>
-              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>213691</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>35615</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="305725" cy="350032"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="TextBox 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2963517" y="242680"/>
-              <a:ext cx="305725" cy="350032"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:f>
-                      <m:fPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:fPr>
-                      <m:num>
-                        <m:r>
-                          <a:rPr lang="ko-KR" altLang="en-US" sz="1100">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>ⅆ</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑌</m:t>
-                        </m:r>
-                      </m:num>
-                      <m:den>
-                        <m:sSup>
-                          <m:sSupPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:sSupPr>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="0">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>ⅆ</m:t>
-                            </m:r>
-                          </m:e>
-                          <m:sup>
-                            <m:r>
-                              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="0">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>2</m:t>
-                            </m:r>
-                          </m:sup>
-                        </m:sSup>
-                        <m:sSub>
-                          <m:sSubPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:sSubPr>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>𝑋</m:t>
-                            </m:r>
-                          </m:e>
-                          <m:sub>
-                            <m:r>
-                              <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>𝑖</m:t>
-                            </m:r>
-                          </m:sub>
-                        </m:sSub>
-                      </m:den>
-                    </m:f>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="TextBox 3"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2963517" y="242680"/>
-              <a:ext cx="305725" cy="350032"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>ⅆ𝑌/(ⅆ^2 𝑋_𝑖 )</a:t>
-              </a:r>
-              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>155712</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>110158</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="397288" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="5" name="TextBox 4">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3592995" y="317223"/>
-              <a:ext cx="397288" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑥</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑖</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                    <m:r>
-                      <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="0">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>+1</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="5" name="TextBox 4"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3592995" y="317223"/>
-              <a:ext cx="397288" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="ko-KR" altLang="en-US" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑥_𝑖+1</a:t>
-              </a:r>
-              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>496956</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>24848</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>182219</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>161324</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>66261</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>186171</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2002,8 +1323,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5052391" y="207066"/>
-          <a:ext cx="4306957" cy="4923823"/>
+          <a:off x="5400260" y="215348"/>
+          <a:ext cx="3859697" cy="4542823"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2493,7 +1814,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="2:6">
@@ -2633,106 +1954,106 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" t="s">
         <v>167</v>
-      </c>
-      <c r="C4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D4" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" t="s">
         <v>173</v>
-      </c>
-      <c r="D5" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D6" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" t="s">
         <v>172</v>
       </c>
-      <c r="C8" t="s">
-        <v>176</v>
-      </c>
       <c r="D8" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D9" t="s">
         <v>176</v>
-      </c>
-      <c r="D9" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C10" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D10" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2758,139 +2079,139 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="2:4">
       <c r="B3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" t="s">
         <v>205</v>
-      </c>
-      <c r="C3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D3" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" t="s">
         <v>205</v>
-      </c>
-      <c r="C4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D4" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5" t="s">
         <v>205</v>
-      </c>
-      <c r="C5" t="s">
-        <v>208</v>
-      </c>
-      <c r="D5" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C8" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" t="s">
         <v>210</v>
       </c>
-      <c r="C9" t="s">
-        <v>214</v>
-      </c>
       <c r="D9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C10" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D10" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C11" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D11" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C12" t="s">
+        <v>213</v>
+      </c>
+      <c r="D12" t="s">
         <v>216</v>
-      </c>
-      <c r="C12" t="s">
-        <v>217</v>
-      </c>
-      <c r="D12" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="13" spans="2:4">
       <c r="B13" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C13" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D13" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2935,7 +2256,7 @@
         <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="45">
@@ -3054,45 +2375,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="30">
-      <c r="B2" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>108</v>
+      <c r="B2" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
         <v>71</v>
       </c>
-      <c r="C4" t="s">
-        <v>75</v>
-      </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:5">
@@ -3100,13 +2421,13 @@
         <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="2:5">
@@ -3114,13 +2435,13 @@
         <v>35</v>
       </c>
       <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
         <v>75</v>
       </c>
-      <c r="D6" t="s">
-        <v>79</v>
-      </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="2:5">
@@ -3128,13 +2449,13 @@
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="2:5">
@@ -3142,13 +2463,13 @@
         <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="2:5">
@@ -3156,13 +2477,13 @@
         <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -3170,13 +2491,13 @@
         <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="2:5">
@@ -3184,186 +2505,186 @@
         <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" t="s">
         <v>89</v>
       </c>
-      <c r="C14" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" t="s">
-        <v>93</v>
-      </c>
       <c r="E14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" t="s">
         <v>87</v>
-      </c>
-      <c r="D16" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E18" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D19" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
         <v>98</v>
       </c>
-      <c r="C20" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" t="s">
-        <v>102</v>
-      </c>
       <c r="E20" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E21" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D22" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E22" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E23" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -3377,7 +2698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3391,409 +2712,409 @@
   <sheetData>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B3" t="s">
         <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B9" t="s">
         <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B14" t="s">
         <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B16" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C16" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D16" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C17" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B18" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D18" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D19" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B20" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B21" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C21" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D21" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B22" t="s">
         <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D22" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B23" t="s">
         <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B24" t="s">
         <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D24" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D25" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C26" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B27" t="s">
         <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D27" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B28" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C28" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D28" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B29" t="s">
         <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D29" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B30" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C30" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D30" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C31" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3827,22 +3148,22 @@
         <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
         <v>43</v>
@@ -3850,13 +3171,13 @@
     </row>
     <row r="4" spans="2:7">
       <c r="B4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E4" t="s">
         <v>44</v>
@@ -3864,13 +3185,13 @@
     </row>
     <row r="5" spans="2:7">
       <c r="B5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E5" t="s">
         <v>45</v>
@@ -3878,13 +3199,13 @@
     </row>
     <row r="6" spans="2:7">
       <c r="B6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E6" t="s">
         <v>47</v>
@@ -3892,13 +3213,13 @@
     </row>
     <row r="7" spans="2:7">
       <c r="B7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E7" t="s">
         <v>46</v>
@@ -3909,10 +3230,10 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E8" t="s">
         <v>48</v>
@@ -3923,10 +3244,10 @@
         <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
         <v>43</v>
@@ -3937,10 +3258,10 @@
         <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E10" t="s">
         <v>49</v>
@@ -3951,10 +3272,10 @@
         <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D11" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E11" t="s">
         <v>44</v>
@@ -3965,10 +3286,10 @@
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E12" t="s">
         <v>45</v>
@@ -3979,10 +3300,10 @@
         <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D13" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E13" t="s">
         <v>50</v>
@@ -3993,10 +3314,10 @@
         <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D14" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E14" t="s">
         <v>47</v>
@@ -4007,10 +3328,10 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E15" t="s">
         <v>46</v>
@@ -4021,10 +3342,10 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
         <v>43</v>
@@ -4035,10 +3356,10 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D17" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E17" t="s">
         <v>51</v>
@@ -4049,10 +3370,10 @@
         <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D18" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E18" t="s">
         <v>52</v>
@@ -4063,10 +3384,10 @@
         <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D19" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E19" t="s">
         <v>44</v>
@@ -4077,10 +3398,10 @@
         <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D20" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E20" t="s">
         <v>53</v>
@@ -4091,10 +3412,10 @@
         <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D21" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E21" t="s">
         <v>45</v>
@@ -4105,10 +3426,10 @@
         <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E22" t="s">
         <v>47</v>
@@ -4119,10 +3440,10 @@
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D23" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E23" t="s">
         <v>57</v>
@@ -4133,10 +3454,10 @@
         <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D24" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E24" t="s">
         <v>46</v>
@@ -4144,13 +3465,13 @@
     </row>
     <row r="25" spans="2:5">
       <c r="B25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D25" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E25" t="s">
         <v>48</v>
@@ -4158,13 +3479,13 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E26" t="s">
         <v>43</v>
@@ -4172,13 +3493,13 @@
     </row>
     <row r="27" spans="2:5">
       <c r="B27" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D27" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E27" t="s">
         <v>55</v>
@@ -4186,13 +3507,13 @@
     </row>
     <row r="28" spans="2:5">
       <c r="B28" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C28" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D28" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E28" t="s">
         <v>52</v>
@@ -4200,13 +3521,13 @@
     </row>
     <row r="29" spans="2:5">
       <c r="B29" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D29" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E29" t="s">
         <v>49</v>
@@ -4214,13 +3535,13 @@
     </row>
     <row r="30" spans="2:5">
       <c r="B30" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C30" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D30" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E30" t="s">
         <v>44</v>
@@ -4228,13 +3549,13 @@
     </row>
     <row r="31" spans="2:5">
       <c r="B31" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D31" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E31" t="s">
         <v>56</v>
@@ -4242,13 +3563,13 @@
     </row>
     <row r="32" spans="2:5">
       <c r="B32" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C32" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D32" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E32" t="s">
         <v>45</v>
@@ -4256,13 +3577,13 @@
     </row>
     <row r="33" spans="2:5">
       <c r="B33" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C33" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D33" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E33" t="s">
         <v>50</v>
@@ -4270,13 +3591,13 @@
     </row>
     <row r="34" spans="2:5">
       <c r="B34" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D34" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E34" t="s">
         <v>47</v>
@@ -4284,13 +3605,13 @@
     </row>
     <row r="35" spans="2:5">
       <c r="B35" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D35" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E35" t="s">
         <v>58</v>
@@ -4298,13 +3619,13 @@
     </row>
     <row r="36" spans="2:5">
       <c r="B36" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D36" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E36" t="s">
         <v>54</v>
@@ -4312,7 +3633,7 @@
     </row>
     <row r="38" spans="2:5">
       <c r="B38" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -4324,319 +3645,308 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B2:F22"/>
+  <dimension ref="B2:F21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="B2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F2" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
+      <c r="B3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.7</v>
+      </c>
+      <c r="D4">
+        <v>-13.19</v>
+      </c>
+      <c r="E4">
+        <v>22.16</v>
+      </c>
+      <c r="F4">
+        <v>1.3</v>
+      </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="10">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1.3</v>
+      </c>
+      <c r="D5">
+        <v>17.850000000000001</v>
+      </c>
+      <c r="E5">
+        <v>52.24</v>
+      </c>
+      <c r="F5">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0.95</v>
+      </c>
+      <c r="D6">
+        <v>-2.72</v>
+      </c>
+      <c r="E6">
+        <v>56.64</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="C5" s="11">
-        <v>0.7</v>
-      </c>
-      <c r="D5" s="12">
-        <v>-13.19</v>
-      </c>
-      <c r="E5" s="12">
-        <v>22.16</v>
-      </c>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="10">
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0.09</v>
+      </c>
+      <c r="E7">
+        <v>60.09</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.6</v>
+      </c>
+      <c r="D9">
+        <v>25.8</v>
+      </c>
+      <c r="E9">
+        <v>-7.68</v>
+      </c>
+      <c r="F9">
+        <v>4.96</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10">
         <v>2</v>
       </c>
-      <c r="C6" s="11">
-        <v>1.3</v>
-      </c>
-      <c r="D6" s="12">
-        <v>17.850000000000001</v>
-      </c>
-      <c r="E6" s="12">
-        <v>52.24</v>
-      </c>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="10">
+      <c r="C10">
+        <v>4.96</v>
+      </c>
+      <c r="D10">
+        <v>16956.16</v>
+      </c>
+      <c r="E10">
+        <v>25498.560000000001</v>
+      </c>
+      <c r="F10">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11">
         <v>3</v>
       </c>
-      <c r="C7" s="11">
-        <v>0.95</v>
-      </c>
-      <c r="D7" s="12">
-        <v>-2.72</v>
-      </c>
-      <c r="E7" s="12">
-        <v>56.64</v>
-      </c>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="10">
+      <c r="C11">
+        <v>4.3</v>
+      </c>
+      <c r="D11">
+        <v>5419.61</v>
+      </c>
+      <c r="E11">
+        <v>10714.92</v>
+      </c>
+      <c r="F11">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12">
         <v>4</v>
       </c>
-      <c r="C8" s="11">
-        <v>1</v>
-      </c>
-      <c r="D8" s="12">
-        <v>0.09</v>
-      </c>
-      <c r="E8" s="12">
-        <v>60.09</v>
-      </c>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="11">
-        <v>1.6</v>
-      </c>
-      <c r="D10" s="12">
-        <v>25.8</v>
-      </c>
-      <c r="E10" s="12">
-        <v>-7.68</v>
-      </c>
-      <c r="F10" s="12">
-        <v>4.96</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="10">
-        <v>2</v>
-      </c>
-      <c r="C11" s="11">
-        <v>4.96</v>
-      </c>
-      <c r="D11" s="12">
-        <v>16956.16</v>
-      </c>
-      <c r="E11" s="12">
-        <v>25498.560000000001</v>
-      </c>
-      <c r="F11" s="12">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12" s="10">
+      <c r="C12">
+        <v>3.79</v>
+      </c>
+      <c r="D12">
+        <v>1696.52</v>
+      </c>
+      <c r="E12">
+        <v>4601.51</v>
+      </c>
+      <c r="F12">
+        <v>3.42</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>3.42</v>
+      </c>
+      <c r="D13">
+        <v>507.53</v>
+      </c>
+      <c r="E13">
+        <v>2070.6</v>
+      </c>
+      <c r="F13">
+        <v>3.18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>3.18</v>
+      </c>
+      <c r="D14">
+        <v>135.68</v>
+      </c>
+      <c r="E14">
+        <v>1036.75</v>
+      </c>
+      <c r="F14">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>3.04</v>
+      </c>
+      <c r="D15">
+        <v>26.45</v>
+      </c>
+      <c r="E15">
+        <v>649.51</v>
+      </c>
+      <c r="F15">
         <v>3</v>
       </c>
-      <c r="C12" s="11">
-        <v>4.3</v>
-      </c>
-      <c r="D12" s="12">
-        <v>5419.61</v>
-      </c>
-      <c r="E12" s="12">
-        <v>10714.92</v>
-      </c>
-      <c r="F12" s="12">
-        <v>3.79</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="10">
-        <v>4</v>
-      </c>
-      <c r="C13" s="11">
-        <v>3.79</v>
-      </c>
-      <c r="D13" s="12">
-        <v>1696.52</v>
-      </c>
-      <c r="E13" s="12">
-        <v>4601.51</v>
-      </c>
-      <c r="F13" s="12">
-        <v>3.42</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="B14" s="10">
-        <v>5</v>
-      </c>
-      <c r="C14" s="11">
-        <v>3.42</v>
-      </c>
-      <c r="D14" s="12">
-        <v>507.53</v>
-      </c>
-      <c r="E14" s="12">
-        <v>2070.6</v>
-      </c>
-      <c r="F14" s="12">
-        <v>3.18</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" s="10">
-        <v>6</v>
-      </c>
-      <c r="C15" s="11">
-        <v>3.18</v>
-      </c>
-      <c r="D15" s="12">
-        <v>135.68</v>
-      </c>
-      <c r="E15" s="12">
-        <v>1036.75</v>
-      </c>
-      <c r="F15" s="12">
-        <v>3.04</v>
-      </c>
     </row>
     <row r="16" spans="2:6">
-      <c r="B16" s="10">
-        <v>7</v>
-      </c>
-      <c r="C16" s="11">
-        <v>3.04</v>
-      </c>
-      <c r="D16" s="12">
-        <v>26.45</v>
-      </c>
-      <c r="E16" s="12">
-        <v>649.51</v>
-      </c>
-      <c r="F16" s="12">
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
         <v>3</v>
       </c>
+      <c r="D16">
+        <v>2.08</v>
+      </c>
+      <c r="E16">
+        <v>548.97</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="10">
-        <v>8</v>
-      </c>
-      <c r="C17" s="11">
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17">
         <v>3</v>
       </c>
-      <c r="D17" s="12">
-        <v>2.08</v>
-      </c>
-      <c r="E17" s="12">
-        <v>548.97</v>
-      </c>
-      <c r="F17" s="12">
+      <c r="D17">
+        <v>0.02</v>
+      </c>
+      <c r="E17">
+        <v>540.07000000000005</v>
+      </c>
+      <c r="F17">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="10">
-        <v>9</v>
-      </c>
-      <c r="C18" s="11">
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
         <v>3</v>
       </c>
-      <c r="D18" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="E18" s="12">
-        <v>540.07000000000005</v>
-      </c>
-      <c r="F18" s="12">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>540</v>
+      </c>
+      <c r="F18">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="10">
-        <v>10</v>
-      </c>
-      <c r="C19" s="11">
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19">
         <v>3</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19">
         <v>0</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19">
         <v>540</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="10">
-        <v>11</v>
-      </c>
-      <c r="C20" s="11">
-        <v>3</v>
-      </c>
-      <c r="D20" s="13">
-        <v>0</v>
-      </c>
-      <c r="E20" s="12">
-        <v>540</v>
-      </c>
-      <c r="F20" s="12">
-        <v>3</v>
-      </c>
-    </row>
     <row r="21" spans="2:6">
-      <c r="C21" s="9"/>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="B22" t="s">
-        <v>67</v>
+      <c r="B21" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B4:F4"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4658,16 +3968,16 @@
   <sheetData>
     <row r="2" spans="2:5">
       <c r="B2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="2:5">
@@ -4728,7 +4038,7 @@
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -4753,10 +4063,10 @@
   <sheetData>
     <row r="2" spans="2:3">
       <c r="B2" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="2:3">
@@ -4793,7 +4103,7 @@
     </row>
     <row r="8" spans="2:3">
       <c r="B8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -4822,92 +4132,92 @@
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C5" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: Tab 2.3 Co-authored-by: Choi, Suein <mychloe00@gmail.com>
</commit_message>
<xml_diff>
--- a/data-raw/fig-tab.xlsx
+++ b/data-raw/fig-tab.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmc\pipetbooks\basic\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E8A0D3-96E6-4052-A426-8D468A4A236A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B539BDE-59EC-4BAE-8869-F3A2FE0C4E2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16" sheetId="1" r:id="rId1"/>
@@ -2224,8 +2224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2273,7 +2273,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G3" s="2">
         <v>8</v>
@@ -2296,7 +2296,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G4" s="2">
         <v>8</v>
@@ -2319,7 +2319,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G5" s="2">
         <v>8</v>
@@ -2342,7 +2342,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2">
         <v>8</v>
@@ -2698,7 +2698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>

</xml_diff>